<commit_message>
Added back transition col
</commit_message>
<xml_diff>
--- a/database/bc_database.xlsx
+++ b/database/bc_database.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t xml:space="preserve">nb</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t xml:space="preserve">MAIN-2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I see.</t>
   </si>
 </sst>
 </file>
@@ -84,7 +87,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0%"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -120,6 +123,12 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="3">
@@ -177,7 +186,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -196,6 +205,10 @@
     </xf>
     <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -218,10 +231,10 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="K13" activeCellId="0" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="44.18"/>
@@ -381,8 +394,8 @@
       <c r="J5" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="K5" s="2" t="s">
-        <v>16</v>
+      <c r="K5" s="5" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added random performance picking
</commit_message>
<xml_diff>
--- a/database/bc_database.xlsx
+++ b/database/bc_database.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
   <si>
     <t xml:space="preserve">nb</t>
   </si>
@@ -55,19 +55,25 @@
     <t xml:space="preserve">Utterance</t>
   </si>
   <si>
-    <t xml:space="preserve">0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Human turn hum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">哦好</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Robot turn hum</t>
+    <t xml:space="preserve">Human turn hum0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">哦好一</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Human turn hum1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">哦好二</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Human turn hum2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">哦好三</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robot turn hum0</t>
   </si>
   <si>
     <t xml:space="preserve">happy</t>
@@ -76,22 +82,91 @@
     <t xml:space="preserve">MAIN-1</t>
   </si>
   <si>
-    <t xml:space="preserve">哦好嘅</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not owned turn hum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transition COL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">好</t>
+    <t xml:space="preserve">哦好嘅一</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Robot turn hum1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">哦好嘅</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">二</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Robot turn hum2</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">哦好嘅</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">三</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Not owned turn hum0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">唔一</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not owned turn hum1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">唔二</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not owned turn hum2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">唔三</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transition COL0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">好一</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transition COL1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">好二</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transition COL2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">好三</t>
   </si>
 </sst>
 </file>
@@ -101,7 +176,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -131,6 +206,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Noto Sans CJK SC"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -174,7 +255,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -184,6 +265,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -204,17 +289,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
+      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="21.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="25.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="29.76"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -253,107 +340,315 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="K2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K2" s="2" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="K3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="1" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="K4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="1" t="n">
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="E3" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="F3" s="1" t="n">
+      <c r="E5" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="F5" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="I3" s="1" t="n">
-        <v>90</v>
-      </c>
-      <c r="J3" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="K3" s="2" t="s">
+      <c r="G5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="J5" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="1" t="n">
+      <c r="D6" s="1" t="n">
         <v>80</v>
       </c>
-      <c r="E4" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="F4" s="1" t="n">
+      <c r="E6" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="F6" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="I4" s="1" t="n">
-        <v>90</v>
-      </c>
-      <c r="J4" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="G6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="J6" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="K6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="I5" s="1" t="n">
-        <v>90</v>
-      </c>
-      <c r="J5" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="K5" s="2" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>23</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="I7" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="J7" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="I8" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="J8" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="I9" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="J9" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="E10" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="I10" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="J10" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="I11" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="J11" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="I12" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="J12" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H13" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="I13" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="J13" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added to the variety of bc
</commit_message>
<xml_diff>
--- a/database/bc_database.xlsx
+++ b/database/bc_database.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="35">
   <si>
     <t xml:space="preserve">nb</t>
   </si>
@@ -58,19 +58,16 @@
     <t xml:space="preserve">Human turn hum0</t>
   </si>
   <si>
-    <t xml:space="preserve">哦好一</t>
+    <t xml:space="preserve">明白</t>
   </si>
   <si>
     <t xml:space="preserve">Human turn hum1</t>
   </si>
   <si>
-    <t xml:space="preserve">哦好二</t>
-  </si>
-  <si>
     <t xml:space="preserve">Human turn hum2</t>
   </si>
   <si>
-    <t xml:space="preserve">哦好三</t>
+    <t xml:space="preserve">哦</t>
   </si>
   <si>
     <t xml:space="preserve">Robot turn hum0</t>
@@ -82,91 +79,52 @@
     <t xml:space="preserve">MAIN-1</t>
   </si>
   <si>
-    <t xml:space="preserve">哦好嘅一</t>
+    <t xml:space="preserve">我諗下</t>
   </si>
   <si>
     <t xml:space="preserve">Robot turn hum1</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">哦好嘅</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">二</t>
-    </r>
+    <t xml:space="preserve">俾我諗下</t>
   </si>
   <si>
     <t xml:space="preserve">Robot turn hum2</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">哦好嘅</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Noto Sans CJK SC"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">三</t>
-    </r>
+    <t xml:space="preserve">嗯，等我諗下</t>
   </si>
   <si>
     <t xml:space="preserve">Not owned turn hum0</t>
   </si>
   <si>
-    <t xml:space="preserve">唔一</t>
+    <t xml:space="preserve">嗯</t>
   </si>
   <si>
     <t xml:space="preserve">Not owned turn hum1</t>
   </si>
   <si>
-    <t xml:space="preserve">唔二</t>
-  </si>
-  <si>
     <t xml:space="preserve">Not owned turn hum2</t>
   </si>
   <si>
-    <t xml:space="preserve">唔三</t>
+    <t xml:space="preserve">好</t>
   </si>
   <si>
     <t xml:space="preserve">Transition COL0</t>
   </si>
   <si>
-    <t xml:space="preserve">好一</t>
+    <t xml:space="preserve">好啊</t>
   </si>
   <si>
     <t xml:space="preserve">Transition COL1</t>
   </si>
   <si>
-    <t xml:space="preserve">好二</t>
+    <t xml:space="preserve">好嘞</t>
   </si>
   <si>
     <t xml:space="preserve">Transition COL2</t>
   </si>
   <si>
-    <t xml:space="preserve">好三</t>
+    <t xml:space="preserve">我聽到</t>
   </si>
 </sst>
 </file>
@@ -292,10 +250,10 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C21" activeCellId="0" sqref="C21"/>
+      <selection pane="topLeft" activeCell="J22" activeCellId="0" sqref="J22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.4765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.4609375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="17.22"/>
@@ -339,7 +297,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
@@ -357,8 +315,8 @@
       <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="3" t="s">
-        <v>14</v>
+      <c r="K3" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -366,21 +324,21 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="D5" s="1" t="n">
         <v>80</v>
@@ -392,30 +350,30 @@
         <v>40</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="J5" s="1" t="n">
+        <v>100</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H5" s="1" t="n">
-        <v>10</v>
-      </c>
-      <c r="I5" s="1" t="n">
-        <v>90</v>
-      </c>
-      <c r="J5" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>80</v>
@@ -427,7 +385,7 @@
         <v>40</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H6" s="1" t="n">
         <v>10</v>
@@ -439,18 +397,18 @@
         <v>100</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D7" s="1" t="n">
         <v>80</v>
@@ -462,7 +420,7 @@
         <v>40</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H7" s="1" t="n">
         <v>10</v>
@@ -474,18 +432,18 @@
         <v>100</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" s="1" t="n">
         <v>80</v>
@@ -497,7 +455,7 @@
         <v>40</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H8" s="1" t="n">
         <v>10</v>
@@ -508,8 +466,8 @@
       <c r="J8" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="K8" s="3" t="s">
-        <v>26</v>
+      <c r="K8" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -517,10 +475,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D9" s="1" t="n">
         <v>80</v>
@@ -532,7 +490,7 @@
         <v>40</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H9" s="1" t="n">
         <v>10</v>
@@ -544,7 +502,7 @@
         <v>100</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -552,10 +510,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D10" s="1" t="n">
         <v>80</v>
@@ -567,7 +525,7 @@
         <v>40</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H10" s="1" t="n">
         <v>10</v>
@@ -578,8 +536,8 @@
       <c r="J10" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="K10" s="3" t="s">
-        <v>30</v>
+      <c r="K10" s="2" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -587,10 +545,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H11" s="1" t="n">
         <v>10</v>
@@ -602,7 +560,7 @@
         <v>100</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -610,10 +568,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H12" s="1" t="n">
         <v>10</v>
@@ -625,18 +583,18 @@
         <v>100</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H13" s="1" t="n">
         <v>10</v>
@@ -648,7 +606,7 @@
         <v>100</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
moving forward on vad setting
</commit_message>
<xml_diff>
--- a/database/bc_database.xlsx
+++ b/database/bc_database.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="48">
   <si>
     <t xml:space="preserve">nb</t>
   </si>
@@ -64,7 +64,35 @@
     <t xml:space="preserve">MAIN-SIT_0-L_offer</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;speak&gt;&lt;prosody rate="60%"&gt;嗯噢&lt;/prosody&gt;&lt;/speak&gt;</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;speak&gt;&lt;prosody rate="</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">80</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">%"&gt;嗯噢&lt;/prosody&gt;&lt;/speak&gt;</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Human turn hum1</t>
@@ -73,7 +101,35 @@
     <t xml:space="preserve">MAIN-SIT_0-B_contrasts_smaller</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;speak&gt;&lt;prosody rate="60%"&gt;哦&lt;/prosody&gt;&lt;/speak&gt;</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;speak&gt;&lt;prosody rate="</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">80</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">%"&gt;哦&lt;/prosody&gt;&lt;/speak&gt;</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Human turn hum2</t>
@@ -165,6 +221,9 @@
     <t xml:space="preserve">Not owned turn hum1</t>
   </si>
   <si>
+    <t xml:space="preserve">&lt;speak&gt;&lt;prosody rate="80%"&gt;哦&lt;/prosody&gt;&lt;/speak&gt;</t>
+  </si>
+  <si>
     <t xml:space="preserve">Not owned turn hum2</t>
   </si>
   <si>
@@ -199,7 +258,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -228,6 +287,12 @@
       <name val="Noto Sans CJK SC"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Noto Sans CJK SC"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -305,7 +370,7 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K13" activeCellId="0" sqref="K13"/>
+      <selection pane="topLeft" activeCell="K9" activeCellId="0" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -773,7 +838,7 @@
         <v>100</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>17</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="19.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -781,7 +846,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -808,7 +873,7 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -835,7 +900,7 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>12</v>
@@ -870,7 +935,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>12</v>
@@ -905,7 +970,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
@@ -932,7 +997,7 @@
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
@@ -959,7 +1024,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>12</v>
@@ -994,7 +1059,7 @@
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>12</v>
@@ -1029,7 +1094,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
final tweak of performance part
</commit_message>
<xml_diff>
--- a/database/bc_database.xlsx
+++ b/database/bc_database.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="49">
   <si>
     <t xml:space="preserve">nb</t>
   </si>
@@ -73,7 +73,7 @@
     <t xml:space="preserve">MAIN-SIT_0-B_contrasts_smaller</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;speak&gt;&lt;prosody rate="80%"&gt;&lt;phoneme alphabet="x-amazon-jyutping" ph="ngo4"&gt;哦&lt;/phoneme&gt;&lt;/prosody&gt;&lt;/speak&gt;</t>
+    <t xml:space="preserve">&lt;speak&gt;&lt;prosody rate="70%"&gt;&lt;phoneme alphabet="x-amazon-jyutping" ph="ngo5"&gt;哦&lt;/phoneme&gt;&lt;/prosody&gt;&lt;/speak&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">Human turn hum2</t>
@@ -82,7 +82,7 @@
     <t xml:space="preserve">MAIN-SIT_1-R_Thanksfor3</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;speak&gt;&lt;prosody rate="100%"&gt;&lt;phoneme alphabet="x-amazon-jyutping" ph="ngo4"&gt;哦&lt;/phoneme&gt;&lt;/prosody&gt;&lt;/speak&gt;</t>
+    <t xml:space="preserve">&lt;speak&gt;&lt;prosody rate="100%"&gt;&lt;phoneme alphabet="x-amazon-jyutping" ph="ngo5"&gt;哦&lt;/phoneme&gt;&lt;/prosody&gt;&lt;/speak&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">Human turn hum3</t>
@@ -100,7 +100,7 @@
     <t xml:space="preserve">MAIN-SIT_0-B_frame_big</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;speak&gt;&lt;prosody rate="100%"&gt;&lt;phoneme alphabet="x-amazon-jyutping" ph="teng1 dou2"&gt;聽到&lt;/phoneme&gt;&lt;/prosody&gt;&lt;/speak&gt;</t>
+    <t xml:space="preserve">&lt;speak&gt;&lt;prosody rate="100%"&gt;&lt;phoneme alphabet="x-amazon-jyutping" ph="teng1"&gt;聽&lt;/phoneme&gt;&lt;phoneme alphabet="x-amazon-jyutping" ph="dou2"&gt;到&lt;/phoneme&gt;&lt;/prosody&gt;&lt;/speak&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">Robot turn hum1</t>
@@ -109,7 +109,7 @@
     <t xml:space="preserve">MAIN-SIT_1-R_Me</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;speak&gt;&lt;prosody rate="100%"&gt;&lt;phoneme alphabet="x-amazon-jyutping" ph="ngo5 teng1 dou2"&gt;我聽到&lt;/phoneme&gt;&lt;/prosody&gt;&lt;/speak&gt;</t>
+    <t xml:space="preserve">&lt;speak&gt;&lt;prosody rate="100%"&gt;&lt;phoneme alphabet="x-amazon-jyutping" ph="ngo5"&gt;我&lt;/phoneme&gt;&lt;phoneme alphabet="x-amazon-jyutping" ph="teng1"&gt;聽&lt;/phoneme&gt;&lt;phoneme alphabet="x-amazon-jyutping" ph="dou2"&gt;到&lt;/phoneme&gt;&lt;/prosody&gt;&lt;/speak&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">Robot turn hum2</t>
@@ -192,6 +192,37 @@
     <t xml:space="preserve">Transition COL5</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;speak&gt;&lt;prosody rate="100%"&gt;&lt;phoneme alphabet="x-amazon-jyutping" ph="ngo5"&gt;我&lt;/phoneme&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">&lt;phoneme alphabet="x-amazon-jyutping" ph="teng1"&gt;聽&lt;/phoneme&gt;&lt;phoneme alphabet="x-amazon-jyutping" ph="dou2"&gt;到&lt;/phoneme&gt;&lt;/prosody&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Noto Sans CJK SC"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;/speak&gt;</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">Transition COL6</t>
   </si>
 </sst>
@@ -202,7 +233,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -231,6 +262,12 @@
       <name val="Noto Sans CJK SC"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Noto Sans CJK SC"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -275,7 +312,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -285,6 +322,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -311,8 +352,8 @@
   </sheetPr>
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K25" activeCellId="0" sqref="K25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.4453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -455,7 +496,7 @@
       <c r="J4" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="3" t="s">
         <v>20</v>
       </c>
     </row>
@@ -486,7 +527,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
@@ -521,7 +562,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="73.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
@@ -552,7 +593,7 @@
       <c r="J7" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="K7" s="3" t="s">
         <v>29</v>
       </c>
     </row>
@@ -622,7 +663,7 @@
       <c r="J9" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="K9" s="3" t="s">
         <v>17</v>
       </c>
     </row>
@@ -649,7 +690,7 @@
       <c r="J10" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="K10" s="3" t="s">
         <v>20</v>
       </c>
     </row>
@@ -711,7 +752,7 @@
       <c r="J12" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="K12" s="3" t="s">
+      <c r="K12" s="4" t="s">
         <v>36</v>
       </c>
     </row>
@@ -781,7 +822,7 @@
       <c r="J14" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="K14" s="3" t="s">
         <v>17</v>
       </c>
     </row>
@@ -808,7 +849,7 @@
       <c r="J15" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="K15" s="3" t="s">
         <v>20</v>
       </c>
     </row>
@@ -905,7 +946,7 @@
       <c r="J18" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="K18" s="2" t="s">
+      <c r="K18" s="3" t="s">
         <v>17</v>
       </c>
     </row>
@@ -932,7 +973,7 @@
       <c r="J19" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="K19" s="2" t="s">
+      <c r="K19" s="3" t="s">
         <v>20</v>
       </c>
     </row>
@@ -963,7 +1004,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
         <v>19</v>
       </c>
@@ -998,7 +1039,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="73.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
         <v>20</v>
       </c>
@@ -1030,7 +1071,7 @@
         <v>100</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1038,7 +1079,7 @@
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>12</v>
@@ -1064,41 +1105,41 @@
       <c r="J23" s="1" t="n">
         <v>100</v>
       </c>
-      <c r="K23" s="3" t="s">
+      <c r="K23" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="3"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="3"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="3"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
+      <c r="A47" s="4"/>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>

</xml_diff>